<commit_message>
added ability to run all models in one go
</commit_message>
<xml_diff>
--- a/Logging/Results_Summary.xlsx
+++ b/Logging/Results_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA0036F-F2E1-B142-BA56-D6B615BE43E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F520A0F-7FC6-8E43-97F9-746EEF4D754A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5160" yWindow="-27440" windowWidth="40100" windowHeight="20480" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>2014/15</t>
   </si>
@@ -94,16 +94,19 @@
     <t>Average</t>
   </si>
   <si>
-    <t>GRU+Attention+day of the year, RSE loss</t>
+    <t>21 days ahead</t>
+  </si>
+  <si>
+    <t>14 days ahead</t>
+  </si>
+  <si>
+    <t>7 days ahead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -148,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -177,30 +180,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -226,8 +209,59 @@
       <diagonal/>
     </border>
     <border>
+      <left style="slantDashDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
+      <right style="slantDashDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="slantDashDot">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="slantDashDot">
         <color auto="1"/>
       </right>
       <top/>
@@ -240,42 +274,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +456,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$G$5</c:f>
+              <c:f>Sheet1!$I$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -424,7 +477,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1EFD-0644-83CC-D269DC742C4E}"/>
+              <c16:uniqueId val="{00000000-86D5-5447-91FD-469A15AEEB6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -454,7 +507,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$8:$G$8</c:f>
+              <c:f>Sheet1!$I$8:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -475,7 +528,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1EFD-0644-83CC-D269DC742C4E}"/>
+              <c16:uniqueId val="{00000001-86D5-5447-91FD-469A15AEEB6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -505,7 +558,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$11:$G$11</c:f>
+              <c:f>Sheet1!$I$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -526,7 +579,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1EFD-0644-83CC-D269DC742C4E}"/>
+              <c16:uniqueId val="{00000002-86D5-5447-91FD-469A15AEEB6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -556,7 +609,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$14:$G$14</c:f>
+              <c:f>Sheet1!$I$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -577,7 +630,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1EFD-0644-83CC-D269DC742C4E}"/>
+              <c16:uniqueId val="{00000003-86D5-5447-91FD-469A15AEEB6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -892,7 +945,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$G$4</c:f>
+              <c:f>Sheet1!$I$4:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -913,7 +966,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C6B-5C47-9F0A-872E43EE5F10}"/>
+              <c16:uniqueId val="{00000000-E6F1-7440-92E9-9C10C74C0B76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -943,7 +996,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$G$7</c:f>
+              <c:f>Sheet1!$I$7:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -964,7 +1017,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2C6B-5C47-9F0A-872E43EE5F10}"/>
+              <c16:uniqueId val="{00000001-E6F1-7440-92E9-9C10C74C0B76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -994,7 +1047,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$G$10</c:f>
+              <c:f>Sheet1!$I$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1015,7 +1068,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2C6B-5C47-9F0A-872E43EE5F10}"/>
+              <c16:uniqueId val="{00000002-E6F1-7440-92E9-9C10C74C0B76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1045,7 +1098,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$13:$G$13</c:f>
+              <c:f>Sheet1!$I$13:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1066,7 +1119,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2C6B-5C47-9F0A-872E43EE5F10}"/>
+              <c16:uniqueId val="{00000003-E6F1-7440-92E9-9C10C74C0B76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1381,7 +1434,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$G$3</c:f>
+              <c:f>Sheet1!$I$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1402,7 +1455,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C46A-194F-AAF6-165FDF1F851E}"/>
+              <c16:uniqueId val="{00000000-FA93-6C43-9E34-BF9E85E3029E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1432,7 +1485,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$G$6</c:f>
+              <c:f>Sheet1!$I$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1453,7 +1506,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C46A-194F-AAF6-165FDF1F851E}"/>
+              <c16:uniqueId val="{00000001-FA93-6C43-9E34-BF9E85E3029E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1483,7 +1536,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$9:$G$9</c:f>
+              <c:f>Sheet1!$I$9:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1504,7 +1557,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C46A-194F-AAF6-165FDF1F851E}"/>
+              <c16:uniqueId val="{00000002-FA93-6C43-9E34-BF9E85E3029E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1534,7 +1587,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$12:$G$12</c:f>
+              <c:f>Sheet1!$I$12:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1555,7 +1608,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-C46A-194F-AAF6-165FDF1F851E}"/>
+              <c16:uniqueId val="{00000003-FA93-6C43-9E34-BF9E85E3029E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3408,23 +3461,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>205946</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>2746</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>444501</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>739141</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA96FB66-FA16-A54D-B221-9D3576A6269E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABB070DF-7EE8-BA45-B770-FABD8EB3489F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3446,23 +3499,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>444501</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>739141</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>104346</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338F45FB-4F96-3D4B-817B-A2B63B6582EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC0ABF33-603B-5B40-94E6-66CF92957370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3484,23 +3537,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>444501</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>739141</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F88C8A5-837B-BD44-A591-BED4DADD84DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{154CDBFA-AA1F-5440-B384-25554D6345D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3820,391 +3873,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E926CF44-9EFA-F64D-B1D5-56632D7362B9}">
-  <dimension ref="B2:I17"/>
+  <dimension ref="B1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="148" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="D1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="20" t="s">
         <v>19</v>
       </c>
+      <c r="I2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="21"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="21">
         <v>1.9325765759873701</v>
       </c>
-      <c r="E3" s="7">
+      <c r="J3" s="5">
         <v>2.1790326571079102</v>
       </c>
-      <c r="F3" s="7">
+      <c r="K3" s="5">
         <v>1.9987902400228601</v>
       </c>
-      <c r="G3" s="7">
+      <c r="L3" s="5">
         <v>3.43553758963114</v>
       </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H5" si="0">AVERAGE(D3:G3)</f>
+      <c r="M3" s="22">
+        <f t="shared" ref="M3:M5" si="0">AVERAGE(I3:L3)</f>
         <v>2.38648426568732</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="N3" s="27">
+        <v>2.4536862337724701</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2.6005809067331098</v>
+      </c>
+      <c r="P3" s="4">
+        <v>2.8639001598796501</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>5.4791577726949301</v>
+      </c>
+      <c r="R3" s="22">
+        <f>AVERAGE(N3:Q3)</f>
+        <v>3.3493312682700402</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="21"/>
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="13"/>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="23"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="23">
         <v>2.9939974833885299</v>
       </c>
-      <c r="E4" s="11">
+      <c r="J4" s="8">
         <v>3.1105951710453601</v>
       </c>
-      <c r="F4" s="10">
+      <c r="K4" s="7">
         <v>2.51926249207298</v>
       </c>
-      <c r="G4" s="11">
+      <c r="L4" s="8">
         <v>5.0925985304313803</v>
       </c>
-      <c r="H4" s="12">
+      <c r="M4" s="24">
         <f t="shared" si="0"/>
         <v>3.4291134192345627</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="N4" s="29">
+        <v>3.6290797922743101</v>
+      </c>
+      <c r="O4" s="7">
+        <v>3.80056395236877</v>
+      </c>
+      <c r="P4" s="7">
+        <v>3.60957034540098</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>10.214759827218</v>
+      </c>
+      <c r="R4" s="33">
+        <f>AVERAGE(N4:Q4)</f>
+        <v>5.3134934793155146</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="22"/>
-      <c r="C5" s="13" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="14"/>
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="25"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="25">
         <v>0.92106934980587896</v>
       </c>
-      <c r="E5" s="15">
+      <c r="J5" s="11">
         <v>0.89138986975171997</v>
       </c>
-      <c r="F5" s="15">
+      <c r="K5" s="11">
         <v>0.902058958299358</v>
       </c>
-      <c r="G5" s="15">
+      <c r="L5" s="11">
         <v>0.95260904725644702</v>
       </c>
-      <c r="H5" s="25">
+      <c r="M5" s="26">
         <f t="shared" si="0"/>
         <v>0.91678180627835093</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="N5" s="34">
+        <v>0.92371708656019702</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0.83245146903846901</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.79460335028259099</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>0.93644920626638195</v>
+      </c>
+      <c r="R5" s="35">
+        <f>AVERAGE(N5:Q5)</f>
+        <v>0.87180527803690966</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="20" t="s">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="27"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="27">
         <v>1.87080596447854</v>
       </c>
-      <c r="E6" s="6">
+      <c r="J6" s="4">
         <v>4.0609339440637102</v>
       </c>
-      <c r="F6" s="6">
+      <c r="K6" s="4">
         <v>2.0707939330591598</v>
       </c>
-      <c r="G6" s="6">
+      <c r="L6" s="4">
         <v>3.8764715799860401</v>
       </c>
-      <c r="H6" s="17">
-        <f>AVERAGE(D6:G6)</f>
+      <c r="M6" s="28">
+        <f t="shared" ref="M6:M14" si="1">AVERAGE(I6:L6)</f>
         <v>2.9697513553968622</v>
       </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="32"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="21"/>
-      <c r="C7" s="9" t="s">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="13"/>
+      <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="29"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="29">
         <v>2.7370637825341202</v>
       </c>
-      <c r="E7" s="10">
+      <c r="J7" s="7">
         <v>4.5986247721409299</v>
       </c>
-      <c r="F7" s="11">
+      <c r="K7" s="8">
         <v>2.5040706574257001</v>
       </c>
-      <c r="G7" s="10">
+      <c r="L7" s="7">
         <v>5.8113440561706202</v>
       </c>
-      <c r="H7" s="18">
-        <f>AVERAGE(D7:G7)</f>
+      <c r="M7" s="30">
+        <f t="shared" si="1"/>
         <v>3.9127758170678426</v>
       </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="33"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="22"/>
-      <c r="C8" s="13" t="s">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="14"/>
+      <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="25"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="25">
         <v>0.91724718224982205</v>
       </c>
-      <c r="E8" s="15">
+      <c r="J8" s="11">
         <v>0.869856961774365</v>
       </c>
-      <c r="F8" s="15">
+      <c r="K8" s="11">
         <v>0.87542685064708403</v>
       </c>
-      <c r="G8" s="15">
+      <c r="L8" s="11">
         <v>0.93756979228410697</v>
       </c>
-      <c r="H8" s="19">
-        <f>AVERAGE(D8:G8)</f>
+      <c r="M8" s="31">
+        <f t="shared" si="1"/>
         <v>0.90002519673884451</v>
       </c>
+      <c r="N8" s="25"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="26"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="21"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="21">
         <v>2.4770045280456499</v>
       </c>
-      <c r="E9" s="6">
+      <c r="J9" s="4">
         <v>2.45786380767822</v>
       </c>
-      <c r="F9" s="6">
+      <c r="K9" s="4">
         <v>2.12629270553589</v>
       </c>
-      <c r="G9" s="6">
+      <c r="L9" s="4">
         <v>5.0992717742919904</v>
       </c>
-      <c r="H9" s="17">
-        <f>AVERAGE(D9:G9)</f>
+      <c r="M9" s="28">
+        <f t="shared" si="1"/>
         <v>3.0401082038879377</v>
       </c>
+      <c r="N9" s="21">
+        <v>2.4683794975280802</v>
+      </c>
+      <c r="O9" s="4">
+        <v>3.3064715862274201</v>
+      </c>
+      <c r="P9" s="4">
+        <v>3.9645948410034202</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>5.0529875755310103</v>
+      </c>
+      <c r="R9" s="32">
+        <f t="shared" ref="R9:R14" si="2">AVERAGE(N9:Q9)</f>
+        <v>3.6981083750724828</v>
+      </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="21"/>
-      <c r="C10" s="9" t="s">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="23"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="23">
         <v>3.9480929374694802</v>
       </c>
-      <c r="E10" s="10">
+      <c r="J10" s="7">
         <v>3.88890409469604</v>
       </c>
-      <c r="F10" s="10">
+      <c r="K10" s="7">
         <v>2.7959105968475302</v>
       </c>
-      <c r="G10" s="10">
+      <c r="L10" s="7">
         <v>10.1773061752319</v>
       </c>
-      <c r="H10" s="18">
-        <f>AVERAGE(D10:G10)</f>
+      <c r="M10" s="30">
+        <f t="shared" si="1"/>
         <v>5.2025534510612381</v>
       </c>
+      <c r="N10" s="23">
+        <v>4.1546812057495099</v>
+      </c>
+      <c r="O10" s="7">
+        <v>5.1696925163268999</v>
+      </c>
+      <c r="P10" s="7">
+        <v>6.0678725242614702</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>10.1069078445435</v>
+      </c>
+      <c r="R10" s="33">
+        <f t="shared" si="2"/>
+        <v>6.3747885227203449</v>
+      </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="22"/>
-      <c r="C11" s="13" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="14"/>
+      <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="25"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="25">
         <v>0.90079660924073202</v>
       </c>
-      <c r="E11" s="15">
+      <c r="J11" s="11">
         <v>0.87801778441290101</v>
       </c>
-      <c r="F11" s="15">
+      <c r="K11" s="11">
         <v>0.83426951267614802</v>
       </c>
-      <c r="G11" s="15">
+      <c r="L11" s="11">
         <v>0.89986450953195596</v>
       </c>
-      <c r="H11" s="19">
-        <f>AVERAGE(D11:G11)</f>
+      <c r="M11" s="31">
+        <f t="shared" si="1"/>
         <v>0.8782371039654342</v>
       </c>
+      <c r="N11" s="25">
+        <v>0.80390128703358199</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0.85597071067498598</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0.64890504349878997</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0.84175833197634597</v>
+      </c>
+      <c r="R11" s="26">
+        <f t="shared" si="2"/>
+        <v>0.78763384329592601</v>
+      </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="21"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="21">
         <v>3.1352093691149299</v>
       </c>
-      <c r="E12" s="6">
+      <c r="J12" s="4">
         <v>2.4399948410449301</v>
       </c>
-      <c r="F12" s="6">
+      <c r="K12" s="4">
         <v>3.69390116022148</v>
       </c>
-      <c r="G12" s="6">
+      <c r="L12" s="4">
         <v>4.9369132120285499</v>
       </c>
-      <c r="H12" s="17">
-        <f>AVERAGE(D12:G12)</f>
+      <c r="M12" s="28">
+        <f t="shared" si="1"/>
         <v>3.5515046456024724</v>
       </c>
+      <c r="N12" s="21">
+        <v>3.8929097211528201</v>
+      </c>
+      <c r="O12" s="5">
+        <v>2.3631493338524101</v>
+      </c>
+      <c r="P12" s="5">
+        <v>2.3799262087836102</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>5.4727374462481997</v>
+      </c>
+      <c r="R12" s="22">
+        <f t="shared" si="2"/>
+        <v>3.5271806775092598</v>
+      </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="21"/>
-      <c r="C13" s="9" t="s">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="13"/>
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="23"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="23">
         <v>4.6189800418171796</v>
       </c>
-      <c r="E13" s="10">
+      <c r="J13" s="7">
         <v>3.6074576252202202</v>
       </c>
-      <c r="F13" s="10">
+      <c r="K13" s="7">
         <v>4.3137126977993203</v>
       </c>
-      <c r="G13" s="10">
+      <c r="L13" s="7">
         <v>9.0892070968884102</v>
       </c>
-      <c r="H13" s="18">
-        <f>AVERAGE(D13:G13)</f>
+      <c r="M13" s="30">
+        <f t="shared" si="1"/>
         <v>5.407339365431282</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="N13" s="23">
+        <v>4.6885878337364204</v>
+      </c>
+      <c r="O13" s="8">
+        <v>3.4152036619106001</v>
+      </c>
+      <c r="P13" s="8">
+        <v>3.4667221308727498</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>8.8031896063792008</v>
+      </c>
+      <c r="R13" s="33">
+        <f t="shared" si="2"/>
+        <v>5.0934258082247421</v>
+      </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="22"/>
-      <c r="C14" s="13" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="14"/>
+      <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="25"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="25">
         <v>0.87613419051441699</v>
       </c>
-      <c r="E14" s="14">
+      <c r="J14" s="10">
         <v>0.89727929595409295</v>
       </c>
-      <c r="F14" s="15">
+      <c r="K14" s="11">
         <v>0.90423473711684899</v>
       </c>
-      <c r="G14" s="15">
+      <c r="L14" s="11">
         <v>0.96213563093856302</v>
       </c>
-      <c r="H14" s="19">
-        <f>AVERAGE(D14:G14)</f>
+      <c r="M14" s="31">
+        <f t="shared" si="1"/>
         <v>0.90994596363098057</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2.1631336582365499</v>
-      </c>
-      <c r="E15" s="6">
-        <v>3.4469696697945702</v>
-      </c>
-      <c r="F15" s="6">
-        <v>2.6261885581656399</v>
-      </c>
-      <c r="G15" s="6">
-        <v>3.5817975582102299</v>
-      </c>
-      <c r="H15" s="23">
-        <f>AVERAGE(D15:G15)</f>
-        <v>2.9545223611017475</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="21"/>
-      <c r="C16" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="10">
-        <v>3.2576168240463801</v>
-      </c>
-      <c r="E16" s="10">
-        <v>5.6844742659742602</v>
-      </c>
-      <c r="F16" s="10">
-        <v>3.9271708084294401</v>
-      </c>
-      <c r="G16" s="10">
-        <v>6.1224931052099603</v>
-      </c>
-      <c r="H16" s="24">
-        <f>AVERAGE(D16:G16)</f>
-        <v>4.7479387509150097</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
-      <c r="C17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0.93264511225937996</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.86164113385739605</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0.91569334009095604</v>
-      </c>
-      <c r="G17" s="14">
-        <v>0.97141794474735399</v>
-      </c>
-      <c r="H17" s="16">
-        <f>AVERAGE(D17:G17)</f>
-        <v>0.92034938273877143</v>
-      </c>
-      <c r="I17" s="26"/>
+      <c r="N14" s="25">
+        <v>0.82892458212153897</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0.86784599075652802</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0.77323543639765602</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0.83897762350197003</v>
+      </c>
+      <c r="R14" s="35">
+        <f t="shared" si="2"/>
+        <v>0.82724590819442323</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="D1:H1"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4252,87 +4506,87 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>43466</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>43467</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>43468</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>43469</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>43470</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>43471</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>43472</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>43473</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>43474</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>43475</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>43476</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>43477</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>43478</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>43479</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>43480</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>43481</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>43482</v>
       </c>
     </row>

</xml_diff>

<commit_message>
big experiment to do
</commit_message>
<xml_diff>
--- a/Logging/Results_Summary.xlsx
+++ b/Logging/Results_Summary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4A27D-5735-9546-B6E8-5AB4D81CF223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1182F2-4B68-A243-B07A-46C1C2BE0ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="21">
   <si>
     <t>2014/15</t>
   </si>
@@ -90,6 +93,12 @@
   </si>
   <si>
     <t>Attention</t>
+  </si>
+  <si>
+    <t>28 Day Lag</t>
+  </si>
+  <si>
+    <t>112 Day Lag</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -404,24 +413,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -447,31 +438,62 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,12 +503,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4033,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E926CF44-9EFA-F64D-B1D5-56632D7362B9}">
   <dimension ref="B1:S14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4044,31 +4063,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="17" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="17" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="18"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="12" t="s">
@@ -4080,10 +4099,10 @@
       <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="12" t="s">
@@ -4095,10 +4114,10 @@
       <c r="L2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="O2" s="12" t="s">
@@ -4110,18 +4129,18 @@
       <c r="Q2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="58" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="15">
         <v>2.2819145937423202</v>
       </c>
       <c r="E3" s="4">
@@ -4133,11 +4152,11 @@
       <c r="G3" s="4">
         <v>5.5311230443332597</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="29">
         <f t="shared" ref="H3:H14" si="0">AVERAGE(D3:G3)</f>
         <v>4.2717608767756676</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="15">
         <v>1.9325765759873701</v>
       </c>
       <c r="J3" s="5">
@@ -4149,11 +4168,11 @@
       <c r="L3" s="5">
         <v>3.43553758963114</v>
       </c>
-      <c r="M3" s="22">
+      <c r="M3" s="16">
         <f t="shared" ref="M3:M5" si="1">AVERAGE(I3:L3)</f>
         <v>2.38648426568732</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="21">
         <v>2.4536862337724701</v>
       </c>
       <c r="O3" s="4">
@@ -4165,21 +4184,21 @@
       <c r="Q3" s="4">
         <v>5.4791577726949301</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="16">
         <f>AVERAGE(N3:Q3)</f>
         <v>3.3493312682700402</v>
       </c>
-      <c r="S3" s="37">
+      <c r="S3" s="31">
         <f t="shared" ref="S3:S5" si="2">AVERAGE(R3,M3,H3)</f>
         <v>3.3358588035776759</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="15"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="17">
         <v>3.5585607031087201</v>
       </c>
       <c r="E4" s="7">
@@ -4191,11 +4210,11 @@
       <c r="G4" s="7">
         <v>9.6505510894466209</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="26">
         <f t="shared" si="0"/>
         <v>6.3772291061532602</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="17">
         <v>2.9939974833885299</v>
       </c>
       <c r="J4" s="8">
@@ -4207,11 +4226,11 @@
       <c r="L4" s="8">
         <v>5.0925985304313803</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="18">
         <f t="shared" si="1"/>
         <v>3.4291134192345627</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="23">
         <v>3.6290797922743101</v>
       </c>
       <c r="O4" s="7">
@@ -4223,21 +4242,21 @@
       <c r="Q4" s="7">
         <v>10.214759827218</v>
       </c>
-      <c r="R4" s="32">
+      <c r="R4" s="26">
         <f>AVERAGE(N4:Q4)</f>
         <v>5.3134934793155146</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="30">
         <f t="shared" si="2"/>
         <v>5.0399453349011125</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="19">
         <v>0.90051848445861404</v>
       </c>
       <c r="E5" s="11">
@@ -4247,11 +4266,11 @@
       <c r="G5" s="11">
         <v>0.91321636449931598</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="28">
         <f t="shared" si="0"/>
         <v>0.87214365257552406</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="19">
         <v>0.92106934980587896</v>
       </c>
       <c r="J5" s="11">
@@ -4263,11 +4282,11 @@
       <c r="L5" s="11">
         <v>0.95260904725644702</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="20">
         <f t="shared" si="1"/>
         <v>0.91678180627835093</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="27">
         <v>0.92371708656019702</v>
       </c>
       <c r="O5" s="11">
@@ -4279,28 +4298,28 @@
       <c r="Q5" s="10">
         <v>0.93644920626638195</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="28">
         <f>AVERAGE(N5:Q5)</f>
         <v>0.87180527803690966</v>
       </c>
-      <c r="S5" s="36">
+      <c r="S5" s="30">
         <f t="shared" si="2"/>
         <v>0.88691024563026166</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27">
+      <c r="H6" s="22"/>
+      <c r="I6" s="21">
         <v>1.87080596447854</v>
       </c>
       <c r="J6" s="4">
@@ -4312,28 +4331,28 @@
       <c r="L6" s="4">
         <v>3.8764715799860401</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="22">
         <f t="shared" ref="M6:M14" si="3">AVERAGE(I6:L6)</f>
         <v>2.9697513553968622</v>
       </c>
-      <c r="N6" s="21"/>
+      <c r="N6" s="15"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="37"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="15"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="29">
+      <c r="H7" s="24"/>
+      <c r="I7" s="23">
         <v>2.7370637825341202</v>
       </c>
       <c r="J7" s="7">
@@ -4345,28 +4364,28 @@
       <c r="L7" s="7">
         <v>5.8113440561706202</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="24">
         <f t="shared" si="3"/>
         <v>3.9127758170678426</v>
       </c>
-      <c r="N7" s="23"/>
+      <c r="N7" s="17"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="37"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="16"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="25">
+      <c r="H8" s="25"/>
+      <c r="I8" s="19">
         <v>0.91724718224982205</v>
       </c>
       <c r="J8" s="11">
@@ -4378,25 +4397,25 @@
       <c r="L8" s="11">
         <v>0.93756979228410697</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="25">
         <f t="shared" si="3"/>
         <v>0.90002519673884451</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="37"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="21">
         <v>1.5074936151504501</v>
       </c>
       <c r="E9" s="5">
@@ -4408,11 +4427,11 @@
       <c r="G9" s="4">
         <v>5.4043288230895996</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="16">
         <f t="shared" si="0"/>
         <v>3.0065049231052399</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="15">
         <v>2.4770045280456499</v>
       </c>
       <c r="J9" s="4">
@@ -4424,11 +4443,11 @@
       <c r="L9" s="4">
         <v>5.0992717742919904</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="22">
         <f t="shared" si="3"/>
         <v>3.0401082038879377</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="15">
         <v>2.4683794975280802</v>
       </c>
       <c r="O9" s="4">
@@ -4440,21 +4459,21 @@
       <c r="Q9" s="4">
         <v>5.0529875755310103</v>
       </c>
-      <c r="R9" s="35">
+      <c r="R9" s="29">
         <f t="shared" ref="R9:R14" si="4">AVERAGE(N9:Q9)</f>
         <v>3.6981083750724828</v>
       </c>
-      <c r="S9" s="36">
-        <f>AVERAGE(R9,M9,H9)</f>
+      <c r="S9" s="30">
+        <f t="shared" ref="S9:S14" si="5">AVERAGE(R9,M9,H9)</f>
         <v>3.2482405006885533</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="23">
         <v>2.3063547611236599</v>
       </c>
       <c r="E10" s="8">
@@ -4466,11 +4485,11 @@
       <c r="G10" s="7">
         <v>10.472530364990201</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="24">
         <f t="shared" si="0"/>
         <v>5.1403400301933226</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="17">
         <v>3.9480929374694802</v>
       </c>
       <c r="J10" s="7">
@@ -4482,11 +4501,11 @@
       <c r="L10" s="7">
         <v>10.1773061752319</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="24">
         <f t="shared" si="3"/>
         <v>5.2025534510612381</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="17">
         <v>4.1546812057495099</v>
       </c>
       <c r="O10" s="7">
@@ -4498,21 +4517,21 @@
       <c r="Q10" s="7">
         <v>10.1069078445435</v>
       </c>
-      <c r="R10" s="32">
+      <c r="R10" s="26">
         <f t="shared" si="4"/>
         <v>6.3747885227203449</v>
       </c>
-      <c r="S10" s="37">
-        <f>AVERAGE(R10,M10,H10)</f>
+      <c r="S10" s="31">
+        <f t="shared" si="5"/>
         <v>5.5725606679916346</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="16"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="27">
         <v>0.93779419882444803</v>
       </c>
       <c r="E11" s="11">
@@ -4524,11 +4543,11 @@
       <c r="G11" s="10">
         <v>0.92471716243579105</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="25">
         <f t="shared" si="0"/>
         <v>0.84243215006334005</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="19">
         <v>0.90079660924073202</v>
       </c>
       <c r="J11" s="11">
@@ -4540,11 +4559,11 @@
       <c r="L11" s="11">
         <v>0.89986450953195596</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="25">
         <f t="shared" si="3"/>
         <v>0.8782371039654342</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="19">
         <v>0.80390128703358199</v>
       </c>
       <c r="O11" s="11">
@@ -4556,23 +4575,23 @@
       <c r="Q11" s="11">
         <v>0.84175833197634597</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="20">
         <f t="shared" si="4"/>
         <v>0.78763384329592601</v>
       </c>
-      <c r="S11" s="37">
-        <f>AVERAGE(R11,M11,H11)</f>
+      <c r="S11" s="31">
+        <f t="shared" si="5"/>
         <v>0.83610103244156664</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="58" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="15">
         <v>2.2342843541831998</v>
       </c>
       <c r="E12" s="4">
@@ -4584,11 +4603,11 @@
       <c r="G12" s="5">
         <v>3.9417979415889999</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="22">
         <f t="shared" si="0"/>
         <v>3.1706249800771049</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="15">
         <v>3.1352093691149299</v>
       </c>
       <c r="J12" s="4">
@@ -4600,11 +4619,11 @@
       <c r="L12" s="4">
         <v>4.9369132120285499</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12" s="22">
         <f t="shared" si="3"/>
         <v>3.5515046456024724</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="15">
         <v>3.8929097211528201</v>
       </c>
       <c r="O12" s="5">
@@ -4616,21 +4635,21 @@
       <c r="Q12" s="4">
         <v>5.4727374462481997</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="16">
         <f t="shared" si="4"/>
         <v>3.5271806775092598</v>
       </c>
-      <c r="S12" s="37">
-        <f>AVERAGE(R12,M12,H12)</f>
+      <c r="S12" s="31">
+        <f t="shared" si="5"/>
         <v>3.4164367677296124</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="15"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="17">
         <v>3.6865908130193499</v>
       </c>
       <c r="E13" s="7">
@@ -4642,11 +4661,11 @@
       <c r="G13" s="8">
         <v>7.0322687289940697</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="18">
         <f t="shared" si="0"/>
         <v>4.7254666687905544</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="17">
         <v>4.6189800418171796</v>
       </c>
       <c r="J13" s="7">
@@ -4658,11 +4677,11 @@
       <c r="L13" s="7">
         <v>9.0892070968884102</v>
       </c>
-      <c r="M13" s="30">
+      <c r="M13" s="24">
         <f t="shared" si="3"/>
         <v>5.407339365431282</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="17">
         <v>4.6885878337364204</v>
       </c>
       <c r="O13" s="8">
@@ -4674,21 +4693,21 @@
       <c r="Q13" s="8">
         <v>8.8031896063792008</v>
       </c>
-      <c r="R13" s="32">
+      <c r="R13" s="26">
         <f t="shared" si="4"/>
         <v>5.0934258082247421</v>
       </c>
-      <c r="S13" s="37">
-        <f>AVERAGE(R13,M13,H13)</f>
+      <c r="S13" s="31">
+        <f t="shared" si="5"/>
         <v>5.0754106141488595</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="16"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="19">
         <v>0.84882376053956199</v>
       </c>
       <c r="E14" s="10">
@@ -4700,11 +4719,11 @@
       <c r="G14" s="11">
         <v>0.88973826560934099</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="25">
         <f t="shared" si="0"/>
         <v>0.85552413512922509</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="19">
         <v>0.87613419051441699</v>
       </c>
       <c r="J14" s="10">
@@ -4716,11 +4735,11 @@
       <c r="L14" s="11">
         <v>0.96213563093856302</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="25">
         <f t="shared" si="3"/>
         <v>0.90994596363098057</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="19">
         <v>0.82892458212153897</v>
       </c>
       <c r="O14" s="10">
@@ -4732,12 +4751,12 @@
       <c r="Q14" s="11">
         <v>0.83897762350197003</v>
       </c>
-      <c r="R14" s="34">
+      <c r="R14" s="28">
         <f t="shared" si="4"/>
         <v>0.82724590819442323</v>
       </c>
-      <c r="S14" s="37">
-        <f>AVERAGE(R14,M14,H14)</f>
+      <c r="S14" s="31">
+        <f t="shared" si="5"/>
         <v>0.86423866898487633</v>
       </c>
     </row>
@@ -4761,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9877B6-3CD4-0D40-B3E5-10B6D8BC7D6D}">
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4773,33 +4792,33 @@
   <sheetData>
     <row r="1" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="53" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="53" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="46" t="s">
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="61" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -4811,10 +4830,10 @@
       <c r="G3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -4826,10 +4845,10 @@
       <c r="L3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="12" t="s">
@@ -4841,19 +4860,19 @@
       <c r="Q3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="46"/>
+      <c r="S3" s="61"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="15">
         <v>2.0899544617147199</v>
       </c>
       <c r="E4" s="5">
@@ -4865,11 +4884,11 @@
       <c r="G4" s="4">
         <v>3.36981557305629</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="29">
         <f>AVERAGE(D4:G4)</f>
         <v>3.3016429012322175</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="15">
         <v>2.27412852691173</v>
       </c>
       <c r="J4" s="5">
@@ -4881,11 +4900,11 @@
       <c r="L4" s="4">
         <v>4.35236288204944</v>
       </c>
-      <c r="M4" s="35">
+      <c r="M4" s="29">
         <f>AVERAGE(I4:L4)</f>
         <v>2.9508763646684049</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="15">
         <v>2.4495279159938099</v>
       </c>
       <c r="O4" s="5">
@@ -4897,21 +4916,21 @@
       <c r="Q4" s="5">
         <v>5.9394268326783601</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="16">
         <f>AVERAGE(N4:Q4)</f>
         <v>3.4954844015806721</v>
       </c>
-      <c r="S4" s="47">
+      <c r="S4" s="36">
         <f t="shared" ref="S4:S11" si="0">AVERAGE(R4,M4,H4)</f>
         <v>3.2493345558270978</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="40"/>
-      <c r="C5" s="41" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="17">
         <v>2.7284758836533598</v>
       </c>
       <c r="E5" s="8">
@@ -4923,11 +4942,11 @@
       <c r="G5" s="7">
         <v>6.1934178193673102</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="18">
         <f t="shared" ref="H5:H12" si="1">AVERAGE(D5:G5)</f>
         <v>4.8381486098387674</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="17">
         <v>3.49749665585141</v>
       </c>
       <c r="J5" s="8">
@@ -4939,11 +4958,11 @@
       <c r="L5" s="7">
         <v>7.0763448503546096</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="26">
         <f t="shared" ref="M5:M12" si="2">AVERAGE(I5:L5)</f>
         <v>4.3572858218495201</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="17">
         <v>3.3256675064777301</v>
       </c>
       <c r="O5" s="8">
@@ -4955,21 +4974,21 @@
       <c r="Q5" s="8">
         <v>10.725709329029099</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="18">
         <f t="shared" ref="R5:R12" si="3">AVERAGE(N5:Q5)</f>
         <v>5.4772979081645499</v>
       </c>
-      <c r="S5" s="48">
+      <c r="S5" s="37">
         <f t="shared" si="0"/>
         <v>4.8909107799509464</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="19">
         <v>0.949315933481924</v>
       </c>
       <c r="E6" s="10">
@@ -4979,11 +4998,11 @@
       <c r="G6" s="10">
         <v>0.98137593342329499</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="28">
         <f t="shared" si="1"/>
         <v>0.96471589440722161</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="19">
         <v>0.92069104615386499</v>
       </c>
       <c r="J6" s="11">
@@ -4995,11 +5014,11 @@
       <c r="L6" s="11">
         <v>0.94352904192007003</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="28">
         <f t="shared" si="2"/>
         <v>0.91123350184636653</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="19">
         <v>0.85495617549254399</v>
       </c>
       <c r="O6" s="10">
@@ -5011,23 +5030,23 @@
       <c r="Q6" s="11">
         <v>0.84405918827187798</v>
       </c>
-      <c r="R6" s="26">
+      <c r="R6" s="20">
         <f t="shared" si="3"/>
         <v>0.83091849890967784</v>
       </c>
-      <c r="S6" s="51">
+      <c r="S6" s="40">
         <f t="shared" si="0"/>
         <v>0.9022892983877554</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="15">
         <v>7.9404439699041101</v>
       </c>
       <c r="E7" s="4">
@@ -5039,11 +5058,11 @@
       <c r="G7" s="5">
         <v>3.27845823636767</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="29">
         <f t="shared" si="1"/>
         <v>4.0469107651396126</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="21">
         <v>1.77612913182787</v>
       </c>
       <c r="J7" s="4">
@@ -5055,11 +5074,11 @@
       <c r="L7" s="5">
         <v>3.2594796230593799</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="16">
         <f t="shared" si="2"/>
         <v>2.6599872046265647</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="21">
         <v>2.0968853300435999</v>
       </c>
       <c r="O7" s="4">
@@ -5071,21 +5090,21 @@
       <c r="Q7" s="4">
         <v>6.3854905092730903</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="29">
         <f t="shared" si="3"/>
         <v>3.8227977945406248</v>
       </c>
-      <c r="S7" s="49">
+      <c r="S7" s="38">
         <f t="shared" si="0"/>
         <v>3.5098985881022671</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="40"/>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="63"/>
+      <c r="C8" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="17">
         <v>10.025978476733499</v>
       </c>
       <c r="E8" s="7">
@@ -5097,11 +5116,11 @@
       <c r="G8" s="8">
         <v>5.3254648797708404</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="26">
         <f t="shared" si="1"/>
         <v>5.5395921662113681</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="23">
         <v>2.5958159709152602</v>
       </c>
       <c r="J8" s="7">
@@ -5113,11 +5132,11 @@
       <c r="L8" s="8">
         <v>4.5356432643851399</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="18">
         <f t="shared" si="2"/>
         <v>3.8431590358955727</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="23">
         <v>3.0660923187743201</v>
       </c>
       <c r="O8" s="7">
@@ -5129,21 +5148,21 @@
       <c r="Q8" s="7">
         <v>11.461019830575999</v>
       </c>
-      <c r="R8" s="32">
+      <c r="R8" s="26">
         <f t="shared" si="3"/>
         <v>6.0479146439860969</v>
       </c>
-      <c r="S8" s="49">
+      <c r="S8" s="38">
         <f t="shared" si="0"/>
         <v>5.1435552820310129</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="11">
         <v>0.921614391281808</v>
       </c>
@@ -5153,11 +5172,11 @@
       <c r="G9" s="11">
         <v>0.94450588597841501</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="20">
         <f t="shared" si="1"/>
         <v>0.92711793680926835</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="27">
         <v>0.94343316482097905</v>
       </c>
       <c r="J9" s="11">
@@ -5169,11 +5188,11 @@
       <c r="L9" s="10">
         <v>0.95098560861129899</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="20">
         <f t="shared" si="2"/>
         <v>0.90084689568894316</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="27">
         <v>0.87424446908523701</v>
       </c>
       <c r="O9" s="11">
@@ -5185,23 +5204,23 @@
       <c r="Q9" s="11">
         <v>0.90281033031136304</v>
       </c>
-      <c r="R9" s="26">
+      <c r="R9" s="20">
         <f t="shared" si="3"/>
         <v>0.84285560256350944</v>
       </c>
-      <c r="S9" s="52">
+      <c r="S9" s="41">
         <f t="shared" si="0"/>
         <v>0.89027347835390691</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="21">
         <v>1.55935943126678</v>
       </c>
       <c r="E10" s="4">
@@ -5213,11 +5232,11 @@
       <c r="G10" s="4">
         <v>4.2935638427734402</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="16">
         <f t="shared" si="1"/>
         <v>2.7522391378879529</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="15">
         <v>1.92396128177643</v>
       </c>
       <c r="J10" s="4">
@@ -5229,11 +5248,11 @@
       <c r="L10" s="4">
         <v>5.5808334350585902</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="29">
         <f t="shared" si="2"/>
         <v>3.190354615449905</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="15">
         <v>3.2772839069366499</v>
       </c>
       <c r="O10" s="4">
@@ -5245,21 +5264,21 @@
       <c r="Q10" s="4">
         <v>6.1368136405944798</v>
       </c>
-      <c r="R10" s="35">
+      <c r="R10" s="29">
         <f t="shared" si="3"/>
         <v>3.8147408962249774</v>
       </c>
-      <c r="S10" s="48">
+      <c r="S10" s="37">
         <f t="shared" si="0"/>
         <v>3.252444883187612</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="63"/>
+      <c r="C11" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="23">
         <v>2.3338332176208501</v>
       </c>
       <c r="E11" s="7">
@@ -5271,11 +5290,11 @@
       <c r="G11" s="7">
         <v>9.6586608886718803</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="26">
         <f t="shared" si="1"/>
         <v>4.9443445801734924</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="17">
         <v>3.1200985908508301</v>
       </c>
       <c r="J11" s="7">
@@ -5287,11 +5306,11 @@
       <c r="L11" s="7">
         <v>10.4426460266113</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="26">
         <f t="shared" si="2"/>
         <v>5.3821711540222097</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="17">
         <v>5.2892155647277797</v>
       </c>
       <c r="O11" s="7">
@@ -5303,88 +5322,1406 @@
       <c r="Q11" s="7">
         <v>12.060351371765099</v>
       </c>
-      <c r="R11" s="32">
+      <c r="R11" s="26">
         <f t="shared" si="3"/>
         <v>6.5950381755828751</v>
       </c>
-      <c r="S11" s="49">
+      <c r="S11" s="38">
         <f t="shared" si="0"/>
         <v>5.6405179699261927</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="65"/>
+      <c r="C12" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="42">
         <v>0.94939639734185199</v>
       </c>
-      <c r="E12" s="57">
+      <c r="E12" s="43">
         <v>0.93010780230136503</v>
       </c>
-      <c r="F12" s="57">
+      <c r="F12" s="43">
         <v>0.82490594776728798</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="43">
         <v>0.90903514383611905</v>
       </c>
-      <c r="H12" s="58">
+      <c r="H12" s="44">
         <f t="shared" si="1"/>
         <v>0.90336132281165593</v>
       </c>
-      <c r="I12" s="59">
+      <c r="I12" s="45">
         <v>0.93270427660932498</v>
       </c>
-      <c r="J12" s="60">
+      <c r="J12" s="46">
         <v>0.91981403979264997</v>
       </c>
-      <c r="K12" s="57">
+      <c r="K12" s="43">
         <v>0.84534874985251296</v>
       </c>
-      <c r="L12" s="57">
+      <c r="L12" s="43">
         <v>0.86416016005563601</v>
       </c>
-      <c r="M12" s="58">
+      <c r="M12" s="44">
         <f t="shared" si="2"/>
         <v>0.8905068065775309</v>
       </c>
-      <c r="N12" s="59">
+      <c r="N12" s="45">
         <v>0.81497967272402805</v>
       </c>
-      <c r="O12" s="57">
+      <c r="O12" s="43">
         <v>0.83222925096673495</v>
       </c>
-      <c r="P12" s="57">
+      <c r="P12" s="43">
         <v>0.79364436050458997</v>
       </c>
-      <c r="Q12" s="60">
+      <c r="Q12" s="46">
         <v>0.94119617190916005</v>
       </c>
-      <c r="R12" s="61">
+      <c r="R12" s="47">
         <f t="shared" si="3"/>
         <v>0.84551236402612828</v>
       </c>
-      <c r="S12" s="50">
+      <c r="S12" s="39">
         <f>AVERAGE(R12,M12,H12)</f>
         <v>0.87979349780510496</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="N2:R2"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F65057-F8D9-5340-9C4E-E5CBE3EA5B75}">
+  <dimension ref="B1:U39"/>
+  <sheetViews>
+    <sheetView zoomScale="118" workbookViewId="0">
+      <selection activeCell="N6" sqref="N4:N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="20" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+    </row>
+    <row r="2" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="48"/>
+      <c r="E2" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="48"/>
+      <c r="E3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="61"/>
+    </row>
+    <row r="4" spans="2:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1.3100742774973</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1.2030422905795799</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.4245660967290801</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2.9318551487560298</v>
+      </c>
+      <c r="I4" s="16">
+        <f>AVERAGE(E4:H4)</f>
+        <v>1.7173844533904976</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1.7300874001979101</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.7342749630129299</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2.09708348518671</v>
+      </c>
+      <c r="M4" s="5">
+        <v>3.8174018183023102</v>
+      </c>
+      <c r="N4" s="16">
+        <f>AVERAGE(J4:M4)</f>
+        <v>2.344711916674965</v>
+      </c>
+      <c r="O4" s="15">
+        <v>2.39589055360873</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2.41522307562377</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>3.0017751661871501</v>
+      </c>
+      <c r="R4" s="5">
+        <v>5.0132207076229998</v>
+      </c>
+      <c r="S4" s="29">
+        <f>AVERAGE(O4:R4)</f>
+        <v>3.206527375760662</v>
+      </c>
+      <c r="T4" s="50">
+        <f t="shared" ref="T4:T11" si="0">AVERAGE(S4,N4,I4)</f>
+        <v>2.4228745819420414</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="69"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17">
+        <v>2.1872034520766102</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1.8439640396892401</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.9678060263089301</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5.3075219676523497</v>
+      </c>
+      <c r="I5" s="18">
+        <f t="shared" ref="I5:I12" si="1">AVERAGE(E5:H5)</f>
+        <v>2.8266238714317824</v>
+      </c>
+      <c r="J5" s="17">
+        <v>2.7442336443931801</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2.83916625490291</v>
+      </c>
+      <c r="L5" s="7">
+        <v>2.88139769782586</v>
+      </c>
+      <c r="M5" s="8">
+        <v>6.6739345871975901</v>
+      </c>
+      <c r="N5" s="18">
+        <f t="shared" ref="N5:N12" si="2">AVERAGE(J5:M5)</f>
+        <v>3.784683046079885</v>
+      </c>
+      <c r="O5" s="17">
+        <v>4.3671321290137701</v>
+      </c>
+      <c r="P5" s="7">
+        <v>3.9514385040378599</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>4.64813740138118</v>
+      </c>
+      <c r="R5" s="8">
+        <v>9.0295787549361997</v>
+      </c>
+      <c r="S5" s="26">
+        <f t="shared" ref="S5:S12" si="3">AVERAGE(O5:R5)</f>
+        <v>5.4990716973422522</v>
+      </c>
+      <c r="T5" s="37">
+        <f t="shared" si="0"/>
+        <v>4.0367928716179726</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="69"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.95392115472583705</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.96594469434404595</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.94937663650700199</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.98313147306495496</v>
+      </c>
+      <c r="I6" s="28">
+        <f t="shared" si="1"/>
+        <v>0.96309348966046004</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0.899365166579703</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.915706329640396</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0.89387289085965904</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0.89387289085965904</v>
+      </c>
+      <c r="N6" s="20">
+        <f t="shared" si="2"/>
+        <v>0.90070431948485419</v>
+      </c>
+      <c r="O6" s="19">
+        <v>0.77516337088452802</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0.85664846077151502</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0.72830612561988195</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0.92899458632353604</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="3"/>
+        <v>0.8222781358998652</v>
+      </c>
+      <c r="T6" s="40">
+        <f t="shared" si="0"/>
+        <v>0.89535864834839307</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="69"/>
+      <c r="C7" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21">
+        <v>1.1421509591133401</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.44421326023132</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3.1233957203399201</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2.4826827559367701</v>
+      </c>
+      <c r="I7" s="29">
+        <f t="shared" si="1"/>
+        <v>2.0481106739053376</v>
+      </c>
+      <c r="J7" s="21">
+        <v>1.57401887600275</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2.1588445071356901</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1.8187007875132799</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3.9885256813269501</v>
+      </c>
+      <c r="N7" s="29">
+        <f t="shared" si="2"/>
+        <v>2.3850224629946677</v>
+      </c>
+      <c r="O7" s="21">
+        <v>1.7248034367059599</v>
+      </c>
+      <c r="P7" s="5">
+        <v>2.2087949951993799</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2.87894484615035</v>
+      </c>
+      <c r="R7" s="4">
+        <v>5.1789605604436302</v>
+      </c>
+      <c r="S7" s="16">
+        <f t="shared" si="3"/>
+        <v>2.9978759596248299</v>
+      </c>
+      <c r="T7" s="51">
+        <f t="shared" si="0"/>
+        <v>2.4770030321749452</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="69"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1.8922362586156301</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2.3138469329932798</v>
+      </c>
+      <c r="G8" s="7">
+        <v>4.0183710496406899</v>
+      </c>
+      <c r="H8" s="8">
+        <v>4.2830303324943904</v>
+      </c>
+      <c r="I8" s="26">
+        <f t="shared" si="1"/>
+        <v>3.1268711434359977</v>
+      </c>
+      <c r="J8" s="23">
+        <v>2.1685363209735899</v>
+      </c>
+      <c r="K8" s="7">
+        <v>2.9410000415839801</v>
+      </c>
+      <c r="L8" s="8">
+        <v>2.5972998013974302</v>
+      </c>
+      <c r="M8" s="7">
+        <v>7.1204901400938203</v>
+      </c>
+      <c r="N8" s="26">
+        <f t="shared" si="2"/>
+        <v>3.7068315760122053</v>
+      </c>
+      <c r="O8" s="23">
+        <v>2.9546475677581099</v>
+      </c>
+      <c r="P8" s="8">
+        <v>3.7351413787868202</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>4.4779669434357903</v>
+      </c>
+      <c r="R8" s="7">
+        <v>9.3227399723305506</v>
+      </c>
+      <c r="S8" s="18">
+        <f t="shared" si="3"/>
+        <v>5.1226239655778176</v>
+      </c>
+      <c r="T8" s="51">
+        <f t="shared" si="0"/>
+        <v>3.985442228342007</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.95129039093960399</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.95774929814817</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.94834174616636402</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.98388930571576805</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="1"/>
+        <v>0.9603176852424764</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0.94417397582945595</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.89706160725887596</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0.88527606764954203</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0.96553763117116298</v>
+      </c>
+      <c r="N9" s="28">
+        <f t="shared" si="2"/>
+        <v>0.92301232047725934</v>
+      </c>
+      <c r="O9" s="27">
+        <v>0.88304202815584198</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0.83681898447624903</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0.70566649502754697</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0.92865615628656595</v>
+      </c>
+      <c r="S9" s="28">
+        <f t="shared" si="3"/>
+        <v>0.83854591598655104</v>
+      </c>
+      <c r="T9" s="52">
+        <f t="shared" si="0"/>
+        <v>0.90729197390209559</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="69"/>
+      <c r="C10" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1.9421848058700599</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.75653612613678</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1.924476146698</v>
+      </c>
+      <c r="H10" s="4">
+        <v>4.9520492553710902</v>
+      </c>
+      <c r="I10" s="29">
+        <f t="shared" si="1"/>
+        <v>2.6438115835189828</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2.7367403507232702</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.4038953781127899</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1.9256944656372099</v>
+      </c>
+      <c r="M10" s="4">
+        <v>4.9135642051696804</v>
+      </c>
+      <c r="N10" s="29">
+        <f t="shared" si="2"/>
+        <v>2.9949735999107374</v>
+      </c>
+      <c r="O10" s="15">
+        <v>2.47538495063782</v>
+      </c>
+      <c r="P10" s="4">
+        <v>4.1530623435974103</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>2.2520513534545898</v>
+      </c>
+      <c r="R10" s="4">
+        <v>5.3289675712585396</v>
+      </c>
+      <c r="S10" s="29">
+        <f t="shared" si="3"/>
+        <v>3.5523665547370897</v>
+      </c>
+      <c r="T10" s="51">
+        <f t="shared" si="0"/>
+        <v>3.063717246055603</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="69"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="17">
+        <v>3.5339386463165301</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2.6848938465118399</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3.4798402786254901</v>
+      </c>
+      <c r="H11" s="7">
+        <v>10.397066116333001</v>
+      </c>
+      <c r="I11" s="26">
+        <f t="shared" si="1"/>
+        <v>5.0239347219467154</v>
+      </c>
+      <c r="J11" s="17">
+        <v>4.4410023689270002</v>
+      </c>
+      <c r="K11" s="7">
+        <v>3.7191207408904998</v>
+      </c>
+      <c r="L11" s="7">
+        <v>3.49504470825195</v>
+      </c>
+      <c r="M11" s="7">
+        <v>10.0702199935913</v>
+      </c>
+      <c r="N11" s="26">
+        <f t="shared" si="2"/>
+        <v>5.4313469529151872</v>
+      </c>
+      <c r="O11" s="17">
+        <v>4.3364553451538104</v>
+      </c>
+      <c r="P11" s="7">
+        <v>6.2726669311523402</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>3.3307702541351301</v>
+      </c>
+      <c r="R11" s="7">
+        <v>10.1623620986938</v>
+      </c>
+      <c r="S11" s="26">
+        <f t="shared" si="3"/>
+        <v>6.0255636572837705</v>
+      </c>
+      <c r="T11" s="51">
+        <f t="shared" si="0"/>
+        <v>5.4936151107152247</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="69"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="45">
+        <v>0.863253834343091</v>
+      </c>
+      <c r="F12" s="43">
+        <v>0.92128683887904905</v>
+      </c>
+      <c r="G12" s="43">
+        <v>0.84864826532541504</v>
+      </c>
+      <c r="H12" s="43">
+        <v>0.869668746215564</v>
+      </c>
+      <c r="I12" s="44">
+        <f t="shared" si="1"/>
+        <v>0.87571442119077969</v>
+      </c>
+      <c r="J12" s="45">
+        <v>0.86891121213804501</v>
+      </c>
+      <c r="K12" s="43">
+        <v>0.83869524258029604</v>
+      </c>
+      <c r="L12" s="43">
+        <v>0.84202874087091795</v>
+      </c>
+      <c r="M12" s="43">
+        <v>0.89094506505740301</v>
+      </c>
+      <c r="N12" s="44">
+        <f t="shared" si="2"/>
+        <v>0.86014506516166545</v>
+      </c>
+      <c r="O12" s="45">
+        <v>0.80345273636349901</v>
+      </c>
+      <c r="P12" s="43">
+        <v>0.67541573032221403</v>
+      </c>
+      <c r="Q12" s="46">
+        <v>0.76623517179102696</v>
+      </c>
+      <c r="R12" s="43">
+        <v>0.91149795195915995</v>
+      </c>
+      <c r="S12" s="44">
+        <f t="shared" si="3"/>
+        <v>0.7891503976089751</v>
+      </c>
+      <c r="T12" s="53">
+        <f>AVERAGE(S12,N12,I12)</f>
+        <v>0.84166996132047345</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="16" t="e">
+        <f>AVERAGE(E13:H13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="16" t="e">
+        <f>AVERAGE(J13:M13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="29" t="e">
+        <f>AVERAGE(O13:R13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13" s="50" t="e">
+        <f t="shared" ref="T13:T20" si="4">AVERAGE(S13,N13,I13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B14" s="69"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="18" t="e">
+        <f t="shared" ref="I14:I21" si="5">AVERAGE(E14:H14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="18" t="e">
+        <f t="shared" ref="N14:N21" si="6">AVERAGE(J14:M14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="17"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="26" t="e">
+        <f t="shared" ref="S14:S21" si="7">AVERAGE(O14:R14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14" s="37" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B15" s="69"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="28" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="28" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="20" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T15" s="40" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" s="54"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B16" s="69"/>
+      <c r="C16" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="29" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="29" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="16" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T16" s="51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="54"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="69"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="26" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="26" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="23"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="18" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T17" s="51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="54"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="69"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="27"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="28" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T18" s="52" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U18" s="54"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="69"/>
+      <c r="C19" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="29" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="29" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="15"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="29" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T19" s="51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="54"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" s="69"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="26" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="26" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="17"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="26" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" s="51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="54"/>
+    </row>
+    <row r="21" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="69"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="45"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="45"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="44" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T21" s="53" t="e">
+        <f>AVERAGE(S21,N21,I21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="54"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="54"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
+      <c r="T24" s="54"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
+      <c r="T25" s="54"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
+      <c r="T26" s="54"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
+      <c r="T27" s="54"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
+      <c r="T30" s="54"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="54"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="54"/>
+    </row>
+    <row r="33" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="54"/>
+    </row>
+    <row r="34" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="54"/>
+    </row>
+    <row r="35" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="54"/>
+      <c r="O35" s="54"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="54"/>
+      <c r="T35" s="54"/>
+    </row>
+    <row r="36" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
+      <c r="S36" s="54"/>
+      <c r="T36" s="54"/>
+    </row>
+    <row r="37" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="54"/>
+      <c r="T37" s="54"/>
+    </row>
+    <row r="38" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="54"/>
+      <c r="S38" s="54"/>
+      <c r="T38" s="54"/>
+    </row>
+    <row r="39" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="54"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="54"/>
+      <c r="P39" s="54"/>
+      <c r="Q39" s="54"/>
+      <c r="R39" s="54"/>
+      <c r="S39" s="54"/>
+      <c r="T39" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="B13:B21"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C7:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E8695-D1EC-E743-BF15-9B94E85F1AAF}">
   <dimension ref="A2:A18"/>
   <sheetViews>

</xml_diff>